<commit_message>
ScopePropertiesMiddleware tests now working.
</commit_message>
<xml_diff>
--- a/test/MiddlewareTests/MiddlewareTests/ScopeProperties/TestJson.xlsx
+++ b/test/MiddlewareTests/MiddlewareTests/ScopeProperties/TestJson.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MitchellDenC\source\repos\EDennis.AspNetCore.Base\test\MiddlewareTests\MiddlewareTests\ScopeProperties\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denmi\source\repos\EDennis.AspNetCore.Base\test\MiddlewareTests\MiddlewareTests\ScopeProperties\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A9AB0ED-EE2F-4EEA-A4EE-B2D38469F131}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E11B4E8-8CE4-486E-BB7F-F62636121611}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="18900" windowHeight="11055" xr2:uid="{914E17DC-A849-42DE-BD5C-694BB7A8109C}"/>
+    <workbookView xWindow="52" yWindow="0" windowWidth="17993" windowHeight="10800" xr2:uid="{914E17DC-A849-42DE-BD5C-694BB7A8109C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="24">
   <si>
     <t>ProjectName</t>
   </si>
@@ -84,15 +84,6 @@
     <t>claim*name=jack&amp;claim*role=admin</t>
   </si>
   <si>
-    <t>header*hdr1=123&amp;header*x-user=jill</t>
-  </si>
-  <si>
-    <t>{"User":"jack","Claims":[{"Type":"name","Value":"jack"},{"Type":"role","Value":"admin"}],"Headers":{"hdr1":["ABC"],"hdr2":["DEF"]}}</t>
-  </si>
-  <si>
-    <t>{"User":"jill","Claims":[{"Type":"role","Value":"user"},{"Type":"group","Value":"456"}],"Headers":{"hdr1":["123"],"x-user":["jill"]}}</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
@@ -106,6 +97,12 @@
   </si>
   <si>
     <t>ScopePropertiesApi</t>
+  </si>
+  <si>
+    <t>{"User":"jack","name":"jack","role":"admin","Host":"localhost","hdr1":"ABC","hdr2":"DEF","X-HostPath":"localhost"}</t>
+  </si>
+  <si>
+    <t>{"User":"jill","role":"user","group":"456","Host":"localhost","hdr1":"123","X-User":"jill"}</t>
   </si>
 </sst>
 </file>
@@ -460,23 +457,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3DF70F6-41B8-4967-A575-80BF52770920}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="9.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="42.7109375" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="18.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.59765625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.86328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.59765625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1328125" style="1"/>
+    <col min="6" max="6" width="9.3984375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="42.73046875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -499,9 +496,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>11</v>
@@ -519,9 +516,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>11</v>
@@ -539,9 +536,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
@@ -556,12 +553,12 @@
         <v>8</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>11</v>
@@ -579,9 +576,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
@@ -596,12 +593,12 @@
         <v>13</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>11</v>
@@ -616,12 +613,12 @@
         <v>8</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>11</v>
@@ -630,18 +627,18 @@
         <v>10</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>11</v>
@@ -650,33 +647,33 @@
         <v>10</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bug in ApplicationPropertiesMiddleware ... all Middleware tests passing.
</commit_message>
<xml_diff>
--- a/test/MiddlewareTests/MiddlewareTests/ScopeProperties/TestJson.xlsx
+++ b/test/MiddlewareTests/MiddlewareTests/ScopeProperties/TestJson.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denmi\source\repos\EDennis.AspNetCore.Base\test\MiddlewareTests\MiddlewareTests\ScopeProperties\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E11B4E8-8CE4-486E-BB7F-F62636121611}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F16E32D-B2FD-4651-8537-31B9F6AF04C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52" yWindow="0" windowWidth="17993" windowHeight="10800" xr2:uid="{914E17DC-A849-42DE-BD5C-694BB7A8109C}"/>
+    <workbookView xWindow="442" yWindow="0" windowWidth="18398" windowHeight="10800" xr2:uid="{914E17DC-A849-42DE-BD5C-694BB7A8109C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,9 +75,6 @@
     <t>Headers</t>
   </si>
   <si>
-    <t>header*hdr1=ABC&amp;header*hdr2=DEF</t>
-  </si>
-  <si>
     <t>claim*role=user&amp;claim*group=456</t>
   </si>
   <si>
@@ -87,22 +84,25 @@
     <t>C</t>
   </si>
   <si>
+    <t>ScopePropertiesApi</t>
+  </si>
+  <si>
+    <t>{"User":"jill"}</t>
+  </si>
+  <si>
     <t>header*hdr1=123&amp;header*X-User=jill</t>
   </si>
   <si>
-    <t>X-User=bob</t>
-  </si>
-  <si>
-    <t>{"User":"bob"}</t>
-  </si>
-  <si>
-    <t>ScopePropertiesApi</t>
-  </si>
-  <si>
-    <t>{"User":"jack","name":"jack","role":"admin","Host":"localhost","hdr1":"ABC","hdr2":"DEF","X-HostPath":"localhost"}</t>
-  </si>
-  <si>
-    <t>{"User":"jill","role":"user","group":"456","Host":"localhost","hdr1":"123","X-User":"jill"}</t>
+    <t>header*hdr1=ABC&amp;header*hdr2=DEF&amp;header*X-User=jack</t>
+  </si>
+  <si>
+    <t>claim*X-User=bob</t>
+  </si>
+  <si>
+    <t>{"User":"jack","name":"jack","role":"admin","Host":"localhost","hdr1":"ABC","hdr2":"DEF","X-EntryPoint":"TestProject","X-HostPath":"localhost","X-User":"jack"}</t>
+  </si>
+  <si>
+    <t>{"User":"jill","role":"user","group":"456","Host":"localhost","hdr1":"123","X-EntryPoint":"TestProject","X-User":"jill"}</t>
   </si>
 </sst>
 </file>
@@ -458,7 +458,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -469,7 +469,7 @@
     <col min="4" max="4" width="12.59765625" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.1328125" style="1"/>
     <col min="6" max="6" width="9.3984375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="42.73046875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="47.59765625" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
@@ -498,7 +498,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>11</v>
@@ -513,12 +513,12 @@
         <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>11</v>
@@ -533,12 +533,12 @@
         <v>13</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
@@ -558,7 +558,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>11</v>
@@ -573,12 +573,12 @@
         <v>12</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
@@ -593,12 +593,12 @@
         <v>13</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>11</v>
@@ -618,7 +618,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>11</v>
@@ -627,18 +627,18 @@
         <v>10</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>11</v>
@@ -647,18 +647,18 @@
         <v>10</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>11</v>
@@ -667,13 +667,13 @@
         <v>10</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>